<commit_message>
added specs for agents assemble
</commit_message>
<xml_diff>
--- a/specs/vzcorp/agentsAssemble/agentsAssemble.xlsx
+++ b/specs/vzcorp/agentsAssemble/agentsAssemble.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vzisiadis\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6858B4-4640-4469-B0C2-C7853F24495B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C494A54-17DB-49EA-9865-BF6469762F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="18000" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Your Estimate" sheetId="1" r:id="rId1"/>

</xml_diff>